<commit_message>
Change format of  Test_HBase_Jaguar.xlsx
</commit_message>
<xml_diff>
--- a/benchmark/against_hbase/Test_HBase_Jaguar.xlsx
+++ b/benchmark/against_hbase/Test_HBase_Jaguar.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15720" tabRatio="500"/>
+    <workbookView xWindow="4520" yWindow="1420" windowWidth="28800" windowHeight="15720" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hbase vs Jaguar" sheetId="2" r:id="rId1"/>
@@ -44,9 +44,6 @@
     <t>Insert Rows</t>
   </si>
   <si>
-    <t>Select Times</t>
-  </si>
-  <si>
     <t>Database Details:</t>
   </si>
   <si>
@@ -66,6 +63,9 @@
   </si>
   <si>
     <t>Time/second</t>
+  </si>
+  <si>
+    <t>Select Records</t>
   </si>
 </sst>
 </file>
@@ -75,7 +75,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -119,6 +119,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -137,19 +144,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -161,9 +169,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -181,6 +186,9 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -190,12 +198,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -471,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -490,368 +504,395 @@
   <sheetData>
     <row r="1" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
     </row>
     <row r="2" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="16"/>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="F3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="7">
+        <v>10000000</v>
+      </c>
+      <c r="B4" s="2">
+        <v>17413</v>
+      </c>
+      <c r="C4" s="6">
+        <f>B4/60</f>
+        <v>290.21666666666664</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="F4" s="7">
+        <v>10000000</v>
+      </c>
+      <c r="G4" s="2">
+        <v>552</v>
+      </c>
+      <c r="H4" s="6">
+        <f>G4/60</f>
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="I4" s="5"/>
+      <c r="K4" s="19">
+        <f>C4/H4</f>
+        <v>31.545289855072465</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K5" s="14"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="F6" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="K6" s="14"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="F7" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="K7" s="14"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="F8" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="K8" s="14"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="F9" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="K9" s="14"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="K10" s="14"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K11" s="14"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="F12" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="K12" s="14"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="K13" s="14"/>
+    </row>
+    <row r="14" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="B14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="4" t="s">
+      <c r="D14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K14" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="7">
+        <v>10000</v>
+      </c>
+      <c r="B15" s="2">
+        <v>64</v>
+      </c>
+      <c r="C15" s="6">
+        <f>B15/60</f>
+        <v>1.0666666666666667</v>
+      </c>
+      <c r="F15" s="7">
+        <v>10000</v>
+      </c>
+      <c r="G15" s="2">
         <v>5</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="9">
-        <v>10000</v>
-      </c>
-      <c r="B4" s="3">
-        <v>64</v>
-      </c>
-      <c r="C4" s="7">
-        <f>B4/60</f>
-        <v>1.0666666666666667</v>
-      </c>
-      <c r="F4" s="9">
-        <v>10000</v>
-      </c>
-      <c r="G4" s="3">
-        <v>5</v>
-      </c>
-      <c r="H4" s="11">
-        <f>G4/60</f>
+      <c r="H15" s="9">
+        <f>G15/60</f>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="I4" s="5"/>
-      <c r="K4" s="6">
-        <f>B4/G4</f>
+      <c r="I15" s="4"/>
+      <c r="K15" s="19">
+        <f>B15/G15</f>
         <v>12.8</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="9">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="7">
         <v>30000</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B16" s="2">
         <v>179</v>
       </c>
-      <c r="C5" s="7">
-        <f t="shared" ref="C5:C8" si="0">B5/60</f>
+      <c r="C16" s="6">
+        <f t="shared" ref="C16:C19" si="0">B16/60</f>
         <v>2.9833333333333334</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F16" s="7">
         <v>30000</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G16" s="2">
         <v>16</v>
       </c>
-      <c r="H5" s="11">
-        <f>G5/60</f>
+      <c r="H16" s="9">
+        <f>G16/60</f>
         <v>0.26666666666666666</v>
       </c>
-      <c r="I5" s="5"/>
-      <c r="K5" s="6">
-        <f t="shared" ref="K5:K8" si="1">B5/G5</f>
+      <c r="I16" s="4"/>
+      <c r="K16" s="19">
+        <f t="shared" ref="K16:K19" si="1">B16/G16</f>
         <v>11.1875</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="9">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="7">
         <v>100000</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B17" s="2">
         <v>596</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C17" s="6">
         <f t="shared" si="0"/>
         <v>9.9333333333333336</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F17" s="7">
         <v>100000</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G17" s="2">
         <v>43</v>
       </c>
-      <c r="H6" s="11">
-        <f>G6/60</f>
+      <c r="H17" s="9">
+        <f>G17/60</f>
         <v>0.71666666666666667</v>
       </c>
-      <c r="I6" s="5"/>
-      <c r="K6" s="6">
+      <c r="I17" s="4"/>
+      <c r="K17" s="19">
         <f t="shared" si="1"/>
         <v>13.86046511627907</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="9">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="7">
         <v>300000</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B18" s="2">
         <v>1782</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C18" s="6">
         <f t="shared" si="0"/>
         <v>29.7</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F18" s="7">
         <v>300000</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G18" s="2">
         <v>142</v>
       </c>
-      <c r="H7" s="11">
-        <f>G7/60</f>
+      <c r="H18" s="9">
+        <f>G18/60</f>
         <v>2.3666666666666667</v>
       </c>
-      <c r="I7" s="5"/>
-      <c r="K7" s="6">
+      <c r="I18" s="4"/>
+      <c r="K18" s="19">
         <f t="shared" si="1"/>
         <v>12.549295774647888</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="9">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="7">
         <v>1000000</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B19" s="2">
         <v>6008</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C19" s="12">
         <f t="shared" si="0"/>
         <v>100.13333333333334</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D19" s="8">
         <v>2628</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F19" s="7">
         <v>1000000</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G19" s="2">
         <v>462</v>
       </c>
-      <c r="H8" s="11">
-        <f>G8/60</f>
+      <c r="H19" s="9">
+        <f>G19/60</f>
         <v>7.7</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I19" s="8">
         <v>1706</v>
       </c>
-      <c r="K8" s="6">
+      <c r="K19" s="19">
         <f t="shared" si="1"/>
         <v>13.004329004329005</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="F10" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="F11" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="F12" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-    </row>
-    <row r="13" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="18" t="s">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="18"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="18"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="F13" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="F17" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="17"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D19" s="1"/>
-      <c r="F19" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K19" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="9">
-        <v>10000000</v>
-      </c>
-      <c r="B20" s="3">
-        <v>17413</v>
-      </c>
-      <c r="C20" s="7">
-        <f>B20/60</f>
-        <v>290.21666666666664</v>
-      </c>
-      <c r="D20" s="3"/>
-      <c r="F20" s="9">
-        <v>10000000</v>
-      </c>
-      <c r="G20" s="3">
-        <v>552</v>
-      </c>
-      <c r="H20" s="7">
-        <f>G20/60</f>
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="I20" s="6"/>
-      <c r="K20" s="6">
-        <f>C20/H20</f>
-        <v>31.545289855072465</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B25" s="15">
+      <c r="B22" s="13">
         <v>42950</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B27" s="12"/>
-      <c r="D27" s="12"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B28" s="12"/>
-      <c r="D28" s="12"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B29" s="12"/>
-      <c r="D29" s="12"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B30" s="12"/>
-      <c r="D30" s="12"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B31" s="12"/>
-      <c r="D31" s="12"/>
+      <c r="B28" s="10"/>
+      <c r="D28" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A12:C13"/>
+    <mergeCell ref="F12:H13"/>
+    <mergeCell ref="F1:H2"/>
     <mergeCell ref="A1:C2"/>
-    <mergeCell ref="F1:H2"/>
-    <mergeCell ref="F17:H18"/>
-    <mergeCell ref="A17:C18"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="F8:H8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>